<commit_message>
dnn lab mandatory part
</commit_message>
<xml_diff>
--- a/audio_labs/time-measurements.xlsx
+++ b/audio_labs/time-measurements.xlsx
@@ -192,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -211,9 +211,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -553,7 +550,7 @@
   <dimension ref="B2:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -566,16 +563,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
       <c r="K2" s="5" t="s">
         <v>1</v>
       </c>
@@ -588,99 +585,99 @@
       <c r="R2" s="7"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="R3" s="3"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="4">
-        <v>99</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="2">
+        <v>99</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <v>4939</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="2">
         <f>2*F4</f>
         <v>9878</v>
       </c>
-      <c r="H4" s="4">
-        <f>F4/$D$22 *1000000</f>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H9" si="0">F4/$D$22 *1000000</f>
         <v>14.8095952023988</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="4">
-        <v>99</v>
-      </c>
-      <c r="L4" s="4" t="s">
+      <c r="K4" s="2">
+        <v>99</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="2">
         <v>2891</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="2">
         <f>2*O4</f>
         <v>5782</v>
       </c>
-      <c r="Q4" s="4">
-        <f>O4/$D$22 *1000000</f>
+      <c r="Q4" s="2">
+        <f t="shared" ref="Q4:Q9" si="1">O4/$D$22 *1000000</f>
         <v>8.6686656671664171</v>
       </c>
       <c r="R4" s="3" t="s">
@@ -688,53 +685,53 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="4">
-        <v>99</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="B5" s="2">
+        <v>99</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <v>1184</v>
       </c>
-      <c r="G5" s="4">
-        <f t="shared" ref="G5:G9" si="0">2*F5</f>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G9" si="2">2*F5</f>
         <v>2368</v>
       </c>
-      <c r="H5" s="4">
-        <f>F5/$D$22 *1000000</f>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
         <v>3.5502248875562219</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="4">
-        <v>99</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" s="4" t="s">
+      <c r="K5" s="2">
+        <v>99</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="2">
         <v>870</v>
       </c>
-      <c r="P5" s="4">
-        <f t="shared" ref="P5:P9" si="1">2*O5</f>
+      <c r="P5" s="2">
+        <f t="shared" ref="P5:P9" si="3">2*O5</f>
         <v>1740</v>
       </c>
-      <c r="Q5" s="4">
-        <f>O5/$D$22 *1000000</f>
+      <c r="Q5" s="2">
+        <f t="shared" si="1"/>
         <v>2.6086956521739131</v>
       </c>
       <c r="R5" s="3" t="s">
@@ -742,53 +739,53 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="4">
-        <v>99</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="B6" s="2">
+        <v>99</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>731</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="2">
+        <f t="shared" si="2"/>
+        <v>1462</v>
+      </c>
+      <c r="H6" s="2">
         <f t="shared" si="0"/>
-        <v>1462</v>
-      </c>
-      <c r="H6" s="4">
-        <f>F6/$D$22 *1000000</f>
         <v>2.1919040479760121</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="4">
-        <v>99</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6" s="4" t="s">
+      <c r="K6" s="2">
+        <v>99</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="2">
         <v>414</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="2">
+        <f t="shared" si="3"/>
+        <v>828</v>
+      </c>
+      <c r="Q6" s="2">
         <f t="shared" si="1"/>
-        <v>828</v>
-      </c>
-      <c r="Q6" s="4">
-        <f>O6/$D$22 *1000000</f>
         <v>1.2413793103448276</v>
       </c>
       <c r="R6" s="3" t="s">
@@ -796,53 +793,53 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="4">
-        <v>99</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="B7" s="2">
+        <v>99</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <v>741</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="2">
+        <f t="shared" si="2"/>
+        <v>1482</v>
+      </c>
+      <c r="H7" s="2">
         <f t="shared" si="0"/>
-        <v>1482</v>
-      </c>
-      <c r="H7" s="4">
-        <f>F7/$D$22 *1000000</f>
         <v>2.2218890554722637</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="4">
-        <v>99</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" s="4" t="s">
+      <c r="K7" s="2">
+        <v>99</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="2">
         <v>423</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="2">
+        <f t="shared" si="3"/>
+        <v>846</v>
+      </c>
+      <c r="Q7" s="2">
         <f t="shared" si="1"/>
-        <v>846</v>
-      </c>
-      <c r="Q7" s="4">
-        <f>O7/$D$22 *1000000</f>
         <v>1.2683658170914542</v>
       </c>
       <c r="R7" s="3" t="s">
@@ -850,53 +847,53 @@
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="4">
+      <c r="B8" s="2">
         <v>175</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="2">
         <v>1102</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="2">
+        <f t="shared" si="2"/>
+        <v>2204</v>
+      </c>
+      <c r="H8" s="2">
         <f t="shared" si="0"/>
-        <v>2204</v>
-      </c>
-      <c r="H8" s="4">
-        <f>F8/$D$22 *1000000</f>
         <v>3.3043478260869561</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="2">
         <v>175</v>
       </c>
-      <c r="L8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M8" s="4" t="s">
+      <c r="L8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="2">
         <v>603</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="2">
+        <f t="shared" si="3"/>
+        <v>1206</v>
+      </c>
+      <c r="Q8" s="2">
         <f t="shared" si="1"/>
-        <v>1206</v>
-      </c>
-      <c r="Q8" s="4">
-        <f>O8/$D$22 *1000000</f>
         <v>1.8080959520239881</v>
       </c>
       <c r="R8" s="3" t="s">
@@ -904,53 +901,53 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="4">
+      <c r="B9" s="2">
         <v>175</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="2">
         <v>1091</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>2182</v>
+      </c>
+      <c r="H9" s="2">
         <f t="shared" si="0"/>
-        <v>2182</v>
-      </c>
-      <c r="H9" s="4">
-        <f>F9/$D$22 *1000000</f>
         <v>3.2713643178410794</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="2">
         <v>175</v>
       </c>
-      <c r="L9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M9" s="4" t="s">
+      <c r="L9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="2">
         <v>593</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="2">
+        <f t="shared" si="3"/>
+        <v>1186</v>
+      </c>
+      <c r="Q9" s="2">
         <f t="shared" si="1"/>
-        <v>1186</v>
-      </c>
-      <c r="Q9" s="4">
-        <f>O9/$D$22 *1000000</f>
         <v>1.7781109445277361</v>
       </c>
       <c r="R9" s="3" t="s">
@@ -958,88 +955,88 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="K12" s="2" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="K12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="L13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="M13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="N13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="8" t="s">
+      <c r="O13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="P13" s="3"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="4">
-        <v>99</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="2">
+        <v>99</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="4">
-        <f>F4-O4</f>
+      <c r="F14" s="2">
+        <f t="shared" ref="F14:F19" si="4">F4-O4</f>
         <v>2048</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="2">
         <f>2*F14</f>
         <v>4096</v>
       </c>
-      <c r="H14" s="4">
-        <f>F14/$D$22 *1000000</f>
+      <c r="H14" s="2">
+        <f t="shared" ref="H14:H19" si="5">F14/$D$22 *1000000</f>
         <v>6.1409295352323836</v>
       </c>
       <c r="I14" s="3" t="s">
@@ -1067,28 +1064,28 @@
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="4">
-        <v>99</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="B15" s="2">
+        <v>99</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="4">
-        <f>F5-O5</f>
+      <c r="F15" s="2">
+        <f t="shared" si="4"/>
         <v>314</v>
       </c>
-      <c r="G15" s="4">
-        <f t="shared" ref="G15:G19" si="2">2*F15</f>
+      <c r="G15" s="2">
+        <f t="shared" ref="G15:G19" si="6">2*F15</f>
         <v>628</v>
       </c>
-      <c r="H15" s="4">
-        <f>F15/$D$22 *1000000</f>
+      <c r="H15" s="2">
+        <f t="shared" si="5"/>
         <v>0.94152923538230882</v>
       </c>
       <c r="I15" s="3" t="s">
@@ -1104,11 +1101,11 @@
         <v>1014</v>
       </c>
       <c r="N15" s="3">
-        <f t="shared" ref="N15:N17" si="3">2*M15</f>
+        <f t="shared" ref="N15:N17" si="7">2*M15</f>
         <v>2028</v>
       </c>
       <c r="O15" s="3">
-        <f t="shared" ref="O15:O17" si="4">M15/$D$22 * 1000000</f>
+        <f t="shared" ref="O15:O17" si="8">M15/$D$22 * 1000000</f>
         <v>3.0404797601199403</v>
       </c>
       <c r="P15" s="3" t="s">
@@ -1116,28 +1113,28 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="4">
-        <v>99</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="B16" s="2">
+        <v>99</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="4">
-        <f>F6-O6</f>
+      <c r="F16" s="2">
+        <f t="shared" si="4"/>
         <v>317</v>
       </c>
-      <c r="G16" s="4">
-        <f t="shared" si="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="6"/>
         <v>634</v>
       </c>
-      <c r="H16" s="4">
-        <f>F16/$D$22 *1000000</f>
+      <c r="H16" s="2">
+        <f t="shared" si="5"/>
         <v>0.95052473763118439</v>
       </c>
       <c r="I16" s="3" t="s">
@@ -1153,40 +1150,40 @@
         <v>1004</v>
       </c>
       <c r="N16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2008</v>
       </c>
       <c r="O16" s="3">
+        <f t="shared" si="8"/>
+        <v>3.0104947526236878</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="2">
+        <v>99</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="2">
         <f t="shared" si="4"/>
-        <v>3.0104947526236878</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="4">
-        <v>99</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="4">
-        <f>F7-O7</f>
         <v>318</v>
       </c>
-      <c r="G17" s="4">
-        <f t="shared" si="2"/>
+      <c r="G17" s="2">
+        <f t="shared" si="6"/>
         <v>636</v>
       </c>
-      <c r="H17" s="4">
-        <f>F17/$D$22 *1000000</f>
+      <c r="H17" s="2">
+        <f t="shared" si="5"/>
         <v>0.95352323838080955</v>
       </c>
       <c r="I17" s="3" t="s">
@@ -1202,69 +1199,69 @@
         <v>1004</v>
       </c>
       <c r="N17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2008</v>
       </c>
       <c r="O17" s="3">
+        <f t="shared" si="8"/>
+        <v>3.0104947526236878</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="2">
+        <v>175</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="2">
         <f t="shared" si="4"/>
-        <v>3.0104947526236878</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="4">
+        <v>499</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="6"/>
+        <v>998</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="5"/>
+        <v>1.4962518740629684</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="2">
         <v>175</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="4">
-        <f>F8-O8</f>
-        <v>499</v>
-      </c>
-      <c r="G18" s="4">
-        <f t="shared" si="2"/>
-        <v>998</v>
-      </c>
-      <c r="H18" s="4">
-        <f>F18/$D$22 *1000000</f>
-        <v>1.4962518740629684</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="4">
-        <v>175</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="4">
-        <f>F9-O9</f>
+      <c r="F19" s="2">
+        <f t="shared" si="4"/>
         <v>498</v>
       </c>
-      <c r="G19" s="4">
-        <f t="shared" si="2"/>
+      <c r="G19" s="2">
+        <f t="shared" si="6"/>
         <v>996</v>
       </c>
-      <c r="H19" s="4">
-        <f>F19/$D$22 *1000000</f>
+      <c r="H19" s="2">
+        <f t="shared" si="5"/>
         <v>1.4932533733133433</v>
       </c>
       <c r="I19" s="3" t="s">

</xml_diff>